<commit_message>
Evaluation of Traffic Matrix for Flow Thinning with modular capacities
Evaluation of Flow Thinning with modular capacities for Traffic Matrix 50%, 75%, 100%, 150%, 200%, 250%
</commit_message>
<xml_diff>
--- a/FlowThinning_modular_capactities_Evaluation_Results.xlsx
+++ b/FlowThinning_modular_capactities_Evaluation_Results.xlsx
@@ -13,13 +13,18 @@
   </bookViews>
   <sheets>
     <sheet name="Flow Thinning_100%" sheetId="6" r:id="rId1"/>
+    <sheet name="FlowThinning_50%" sheetId="7" r:id="rId2"/>
+    <sheet name="FlowThinning_75%" sheetId="8" r:id="rId3"/>
+    <sheet name="FlowThinning_150%" sheetId="9" r:id="rId4"/>
+    <sheet name="FlowThinning_200%" sheetId="10" r:id="rId5"/>
+    <sheet name="FlowThinning_250%" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="37">
   <si>
     <t>IP Links</t>
   </si>
@@ -283,7 +288,172 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="36">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -331,7 +501,72 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:D34" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:D34" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="A1:D34"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="IP Links" dataDxfId="33" dataCellStyle="Neutral"/>
+    <tableColumn id="2" name="Working capacity of IP link e [Gbit/s]:" dataDxfId="32"/>
+    <tableColumn id="3" name="Nominal capacity of IP link e in failure free mode [Gbit/s]:" dataDxfId="31"/>
+    <tableColumn id="4" name="Spare capacity of IP link e [Gbit/s]:" dataDxfId="30"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table62" displayName="Table62" ref="A1:D34" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A1:D34"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="IP Links" dataDxfId="27" dataCellStyle="Neutral"/>
+    <tableColumn id="2" name="Working capacity of IP link e [Gbit/s]:" dataDxfId="26"/>
+    <tableColumn id="3" name="Nominal capacity of IP link e in failure free mode [Gbit/s]:" dataDxfId="25"/>
+    <tableColumn id="4" name="Spare capacity of IP link e [Gbit/s]:" dataDxfId="24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table623" displayName="Table623" ref="A1:D34" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:D34"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="IP Links" dataDxfId="21" dataCellStyle="Neutral"/>
+    <tableColumn id="2" name="Working capacity of IP link e [Gbit/s]:" dataDxfId="20"/>
+    <tableColumn id="3" name="Nominal capacity of IP link e in failure free mode [Gbit/s]:" dataDxfId="19"/>
+    <tableColumn id="4" name="Spare capacity of IP link e [Gbit/s]:" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table6234" displayName="Table6234" ref="A1:D34" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:D34"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="IP Links" dataDxfId="15" dataCellStyle="Neutral"/>
+    <tableColumn id="2" name="Working capacity of IP link e [Gbit/s]:" dataDxfId="14"/>
+    <tableColumn id="3" name="Nominal capacity of IP link e in failure free mode [Gbit/s]:" dataDxfId="13"/>
+    <tableColumn id="4" name="Spare capacity of IP link e [Gbit/s]:" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table62345" displayName="Table62345" ref="A1:D34" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:D34"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="IP Links" dataDxfId="9" dataCellStyle="Neutral"/>
+    <tableColumn id="2" name="Working capacity of IP link e [Gbit/s]:" dataDxfId="8"/>
+    <tableColumn id="3" name="Nominal capacity of IP link e in failure free mode [Gbit/s]:" dataDxfId="7"/>
+    <tableColumn id="4" name="Spare capacity of IP link e [Gbit/s]:" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table623456" displayName="Table623456" ref="A1:D34" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D34"/>
   <tableColumns count="4">
     <tableColumn id="1" name="IP Links" dataDxfId="3" dataCellStyle="Neutral"/>
@@ -630,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1150,4 +1385,2609 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.453125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8">
+        <v>300</v>
+      </c>
+      <c r="C2" s="8">
+        <v>300</v>
+      </c>
+      <c r="D2" s="7">
+        <f>C2-B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="8">
+        <v>100</v>
+      </c>
+      <c r="C3" s="8">
+        <v>100</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D32" si="0">C3-B3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="8">
+        <v>100</v>
+      </c>
+      <c r="C4" s="8">
+        <v>100</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="8">
+        <v>100</v>
+      </c>
+      <c r="C5" s="8">
+        <v>100</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8">
+        <v>200</v>
+      </c>
+      <c r="C6" s="8">
+        <v>200</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="8">
+        <v>299.99999999999989</v>
+      </c>
+      <c r="C7" s="8">
+        <v>299.99999999999989</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="8">
+        <v>150</v>
+      </c>
+      <c r="C8" s="8">
+        <v>150</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="8">
+        <v>150</v>
+      </c>
+      <c r="C9" s="8">
+        <v>150</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="8">
+        <v>150</v>
+      </c>
+      <c r="C10" s="8">
+        <v>150</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="8">
+        <v>100</v>
+      </c>
+      <c r="C11" s="8">
+        <v>100</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="8">
+        <v>100</v>
+      </c>
+      <c r="C12" s="8">
+        <v>100</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="8">
+        <v>200</v>
+      </c>
+      <c r="C13" s="8">
+        <v>200</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="8">
+        <v>100</v>
+      </c>
+      <c r="C14" s="8">
+        <v>100</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="8">
+        <v>450</v>
+      </c>
+      <c r="C15" s="8">
+        <v>450</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="8">
+        <v>200</v>
+      </c>
+      <c r="C16" s="8">
+        <v>200</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="8">
+        <v>250</v>
+      </c>
+      <c r="C17" s="8">
+        <v>250</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="8">
+        <v>250</v>
+      </c>
+      <c r="C18" s="8">
+        <v>250</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="8">
+        <v>600</v>
+      </c>
+      <c r="C19" s="8">
+        <v>600</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="8">
+        <v>599.99999999999989</v>
+      </c>
+      <c r="C20" s="8">
+        <v>599.99999999999989</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="8">
+        <v>700.00000000000011</v>
+      </c>
+      <c r="C21" s="8">
+        <v>700.00000000000011</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="8">
+        <v>150</v>
+      </c>
+      <c r="C22" s="8">
+        <v>150</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="8">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="C23" s="8">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="8">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="C24" s="8">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="8">
+        <v>100</v>
+      </c>
+      <c r="C25" s="8">
+        <v>100</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="8">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="C26" s="8">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="8">
+        <v>100</v>
+      </c>
+      <c r="C27" s="8">
+        <v>100</v>
+      </c>
+      <c r="D27" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="8">
+        <v>99.999999999999972</v>
+      </c>
+      <c r="C28" s="8">
+        <v>99.999999999999972</v>
+      </c>
+      <c r="D28" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="8">
+        <v>100</v>
+      </c>
+      <c r="C29" s="8">
+        <v>100</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="8">
+        <v>100</v>
+      </c>
+      <c r="C30" s="8">
+        <v>100</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="8">
+        <v>100</v>
+      </c>
+      <c r="C31" s="8">
+        <v>100</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="8">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="C32" s="8">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="1">
+        <f>SUM(B2:B32)</f>
+        <v>6250</v>
+      </c>
+      <c r="D33" s="1">
+        <f>SUBTOTAL(109,D2:D32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.453125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8">
+        <v>500</v>
+      </c>
+      <c r="C2" s="8">
+        <v>500</v>
+      </c>
+      <c r="D2" s="7">
+        <f>C2-B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="8">
+        <v>100</v>
+      </c>
+      <c r="C3" s="8">
+        <v>100</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D32" si="0">C3-B3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="8">
+        <v>100</v>
+      </c>
+      <c r="C4" s="8">
+        <v>100</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="8">
+        <v>100</v>
+      </c>
+      <c r="C5" s="8">
+        <v>100</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8">
+        <v>300</v>
+      </c>
+      <c r="C6" s="8">
+        <v>300</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="8">
+        <v>400</v>
+      </c>
+      <c r="C7" s="8">
+        <v>400</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="8">
+        <v>250</v>
+      </c>
+      <c r="C8" s="8">
+        <v>250</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="8">
+        <v>300</v>
+      </c>
+      <c r="C9" s="8">
+        <v>300</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="8">
+        <v>200</v>
+      </c>
+      <c r="C10" s="8">
+        <v>200</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="8">
+        <v>150</v>
+      </c>
+      <c r="C11" s="8">
+        <v>150</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="8">
+        <v>250</v>
+      </c>
+      <c r="C12" s="8">
+        <v>250</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="8">
+        <v>300</v>
+      </c>
+      <c r="C13" s="8">
+        <v>300</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="8">
+        <v>100</v>
+      </c>
+      <c r="C14" s="8">
+        <v>100</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="8">
+        <v>650</v>
+      </c>
+      <c r="C15" s="8">
+        <v>650</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="8">
+        <v>300</v>
+      </c>
+      <c r="C16" s="8">
+        <v>300</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="8">
+        <v>350</v>
+      </c>
+      <c r="C17" s="8">
+        <v>350</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="8">
+        <v>400</v>
+      </c>
+      <c r="C18" s="8">
+        <v>400</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="8">
+        <v>900</v>
+      </c>
+      <c r="C19" s="8">
+        <v>900</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="8">
+        <v>900</v>
+      </c>
+      <c r="C20" s="8">
+        <v>900</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1050</v>
+      </c>
+      <c r="C21" s="8">
+        <v>1050</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="8">
+        <v>200</v>
+      </c>
+      <c r="C22" s="8">
+        <v>200</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="8">
+        <v>100</v>
+      </c>
+      <c r="C23" s="8">
+        <v>100</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="8">
+        <v>100</v>
+      </c>
+      <c r="C24" s="8">
+        <v>100</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="8">
+        <v>100</v>
+      </c>
+      <c r="C25" s="8">
+        <v>100</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="8">
+        <v>100</v>
+      </c>
+      <c r="C26" s="8">
+        <v>100</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="8">
+        <v>100</v>
+      </c>
+      <c r="C27" s="8">
+        <v>100</v>
+      </c>
+      <c r="D27" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="8">
+        <v>150</v>
+      </c>
+      <c r="C28" s="8">
+        <v>150</v>
+      </c>
+      <c r="D28" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="8">
+        <v>100</v>
+      </c>
+      <c r="C29" s="8">
+        <v>100</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="8">
+        <v>100</v>
+      </c>
+      <c r="C30" s="8">
+        <v>100</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="8">
+        <v>100</v>
+      </c>
+      <c r="C31" s="8">
+        <v>100</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="8">
+        <v>100</v>
+      </c>
+      <c r="C32" s="8">
+        <v>100</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="1">
+        <f>SUM(B2:B32)</f>
+        <v>8850</v>
+      </c>
+      <c r="D33" s="1">
+        <f>SUBTOTAL(109,D2:D32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.453125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8">
+        <v>900</v>
+      </c>
+      <c r="C2" s="8">
+        <v>900</v>
+      </c>
+      <c r="D2" s="7">
+        <f>C2-B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="8">
+        <v>250</v>
+      </c>
+      <c r="C3" s="8">
+        <v>250</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D32" si="0">C3-B3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="8">
+        <v>150</v>
+      </c>
+      <c r="C4" s="8">
+        <v>150</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="8">
+        <v>300</v>
+      </c>
+      <c r="C5" s="8">
+        <v>300</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8">
+        <v>600</v>
+      </c>
+      <c r="C6" s="8">
+        <v>600</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="8">
+        <v>850</v>
+      </c>
+      <c r="C7" s="8">
+        <v>850</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="8">
+        <v>450</v>
+      </c>
+      <c r="C8" s="8">
+        <v>450</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="8">
+        <v>500</v>
+      </c>
+      <c r="C9" s="8">
+        <v>500</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="8">
+        <v>400</v>
+      </c>
+      <c r="C10" s="8">
+        <v>400</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="8">
+        <v>300</v>
+      </c>
+      <c r="C11" s="8">
+        <v>300</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="8">
+        <v>300</v>
+      </c>
+      <c r="C12" s="8">
+        <v>300</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="8">
+        <v>550</v>
+      </c>
+      <c r="C13" s="8">
+        <v>550</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="8">
+        <v>100</v>
+      </c>
+      <c r="C14" s="8">
+        <v>100</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="8">
+        <v>1300</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1300</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="8">
+        <v>600</v>
+      </c>
+      <c r="C16" s="8">
+        <v>600</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="8">
+        <v>700</v>
+      </c>
+      <c r="C17" s="8">
+        <v>700</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="8">
+        <v>750</v>
+      </c>
+      <c r="C18" s="8">
+        <v>750</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1800</v>
+      </c>
+      <c r="C19" s="8">
+        <v>1800</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="8">
+        <v>1750</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1750</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="8">
+        <v>2100</v>
+      </c>
+      <c r="C21" s="8">
+        <v>2100</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="8">
+        <v>450</v>
+      </c>
+      <c r="C22" s="8">
+        <v>450</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="8">
+        <v>200</v>
+      </c>
+      <c r="C23" s="8">
+        <v>200</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="8">
+        <v>100</v>
+      </c>
+      <c r="C24" s="8">
+        <v>100</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="8">
+        <v>100</v>
+      </c>
+      <c r="C25" s="8">
+        <v>100</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="8">
+        <v>250</v>
+      </c>
+      <c r="C26" s="8">
+        <v>250</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="8">
+        <v>250</v>
+      </c>
+      <c r="C27" s="8">
+        <v>250</v>
+      </c>
+      <c r="D27" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="8">
+        <v>250</v>
+      </c>
+      <c r="C28" s="8">
+        <v>250</v>
+      </c>
+      <c r="D28" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="8">
+        <v>200</v>
+      </c>
+      <c r="C29" s="8">
+        <v>200</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="8">
+        <v>100</v>
+      </c>
+      <c r="C30" s="8">
+        <v>100</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="8">
+        <v>250</v>
+      </c>
+      <c r="C31" s="8">
+        <v>250</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="8">
+        <v>100</v>
+      </c>
+      <c r="C32" s="8">
+        <v>100</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="1">
+        <f>SUM(B2:B32)</f>
+        <v>16900</v>
+      </c>
+      <c r="D33" s="1">
+        <f>SUBTOTAL(109,D2:D32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.453125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1450</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1450</v>
+      </c>
+      <c r="D2" s="7">
+        <f>C2-B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="8">
+        <v>300</v>
+      </c>
+      <c r="C3" s="8">
+        <v>300</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D32" si="0">C3-B3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="8">
+        <v>150</v>
+      </c>
+      <c r="C4" s="8">
+        <v>150</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="8">
+        <v>300</v>
+      </c>
+      <c r="C5" s="8">
+        <v>300</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8">
+        <v>750</v>
+      </c>
+      <c r="C6" s="8">
+        <v>750</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="8">
+        <v>1200</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1200</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="8">
+        <v>600</v>
+      </c>
+      <c r="C8" s="8">
+        <v>600</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="8">
+        <v>600</v>
+      </c>
+      <c r="C9" s="8">
+        <v>600</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="8">
+        <v>600</v>
+      </c>
+      <c r="C10" s="8">
+        <v>600</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="8">
+        <v>300</v>
+      </c>
+      <c r="C11" s="8">
+        <v>300</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="8">
+        <v>450</v>
+      </c>
+      <c r="C12" s="8">
+        <v>450</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="8">
+        <v>750</v>
+      </c>
+      <c r="C13" s="8">
+        <v>750</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="8">
+        <v>100</v>
+      </c>
+      <c r="C14" s="8">
+        <v>100</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="8">
+        <v>1800</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1800</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="8">
+        <v>850</v>
+      </c>
+      <c r="C16" s="8">
+        <v>850</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="8">
+        <v>900</v>
+      </c>
+      <c r="C17" s="8">
+        <v>900</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1000</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="8">
+        <v>2400</v>
+      </c>
+      <c r="C19" s="8">
+        <v>2400</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="8">
+        <v>2400</v>
+      </c>
+      <c r="C20" s="8">
+        <v>2400</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="8">
+        <v>2850</v>
+      </c>
+      <c r="C21" s="8">
+        <v>2850</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="8">
+        <v>600</v>
+      </c>
+      <c r="C22" s="8">
+        <v>600</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="8">
+        <v>250</v>
+      </c>
+      <c r="C23" s="8">
+        <v>250</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="8">
+        <v>100</v>
+      </c>
+      <c r="C24" s="8">
+        <v>100</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="8">
+        <v>100</v>
+      </c>
+      <c r="C25" s="8">
+        <v>100</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="8">
+        <v>300</v>
+      </c>
+      <c r="C26" s="8">
+        <v>300</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="8">
+        <v>300</v>
+      </c>
+      <c r="C27" s="8">
+        <v>300</v>
+      </c>
+      <c r="D27" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="8">
+        <v>300</v>
+      </c>
+      <c r="C28" s="8">
+        <v>300</v>
+      </c>
+      <c r="D28" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="8">
+        <v>300</v>
+      </c>
+      <c r="C29" s="8">
+        <v>300</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="8">
+        <v>150</v>
+      </c>
+      <c r="C30" s="8">
+        <v>150</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="8">
+        <v>300</v>
+      </c>
+      <c r="C31" s="8">
+        <v>300</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="8">
+        <v>150</v>
+      </c>
+      <c r="C32" s="8">
+        <v>150</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="1">
+        <f>SUM(B2:B32)</f>
+        <v>22600</v>
+      </c>
+      <c r="D33" s="1">
+        <f>SUBTOTAL(109,D2:D32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.453125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1800</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1800</v>
+      </c>
+      <c r="D2" s="7">
+        <f>C2-B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="8">
+        <v>400</v>
+      </c>
+      <c r="C3" s="8">
+        <v>400</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D32" si="0">C3-B3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="8">
+        <v>200</v>
+      </c>
+      <c r="C4" s="8">
+        <v>200</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="8">
+        <v>300</v>
+      </c>
+      <c r="C5" s="8">
+        <v>300</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="8">
+        <v>1500</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1500</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="8">
+        <v>850</v>
+      </c>
+      <c r="C8" s="8">
+        <v>850</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="8">
+        <v>900</v>
+      </c>
+      <c r="C9" s="8">
+        <v>900</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="8">
+        <v>700</v>
+      </c>
+      <c r="C10" s="8">
+        <v>700</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="8">
+        <v>300</v>
+      </c>
+      <c r="C11" s="8">
+        <v>300</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="8">
+        <v>900</v>
+      </c>
+      <c r="C12" s="8">
+        <v>900</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="8">
+        <v>900</v>
+      </c>
+      <c r="C13" s="8">
+        <v>900</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="8">
+        <v>100</v>
+      </c>
+      <c r="C14" s="8">
+        <v>100</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="8">
+        <v>2100</v>
+      </c>
+      <c r="C15" s="8">
+        <v>2100</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1000</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1150</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1150</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="8">
+        <v>1250</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1250</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="8">
+        <v>3000</v>
+      </c>
+      <c r="C19" s="8">
+        <v>3000</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="8">
+        <v>3300</v>
+      </c>
+      <c r="C20" s="8">
+        <v>3300</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="8">
+        <v>3600</v>
+      </c>
+      <c r="C21" s="8">
+        <v>3600</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="8">
+        <v>800</v>
+      </c>
+      <c r="C22" s="8">
+        <v>800</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="8">
+        <v>300</v>
+      </c>
+      <c r="C23" s="8">
+        <v>300</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="8">
+        <v>100</v>
+      </c>
+      <c r="C24" s="8">
+        <v>100</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="8">
+        <v>150</v>
+      </c>
+      <c r="C25" s="8">
+        <v>150</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="8">
+        <v>300</v>
+      </c>
+      <c r="C26" s="8">
+        <v>300</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="8">
+        <v>300</v>
+      </c>
+      <c r="C27" s="8">
+        <v>300</v>
+      </c>
+      <c r="D27" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="8">
+        <v>300</v>
+      </c>
+      <c r="C28" s="8">
+        <v>300</v>
+      </c>
+      <c r="D28" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="8">
+        <v>300</v>
+      </c>
+      <c r="C29" s="8">
+        <v>300</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="8">
+        <v>100</v>
+      </c>
+      <c r="C30" s="8">
+        <v>100</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="8">
+        <v>300</v>
+      </c>
+      <c r="C31" s="8">
+        <v>300</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="8">
+        <v>100</v>
+      </c>
+      <c r="C32" s="8">
+        <v>100</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="1">
+        <f>SUM(B2:B32)</f>
+        <v>28300</v>
+      </c>
+      <c r="D33" s="1">
+        <f>SUBTOTAL(109,D2:D32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>